<commit_message>
Retraining the F_Cristan XGB model
</commit_message>
<xml_diff>
--- a/RAAL/Production/Input/GHI_2024-02-15.xlsx
+++ b/RAAL/Production/Input/GHI_2024-02-15.xlsx
@@ -1,16 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mynexte-my.sharepoint.com/personal/andrei_ionita_mynexte_com/Documents/Desktop/ML/Forecast_app/RAAL/Production/Input/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_9EA18A5EAD349073E0551F7C138D1B4A422A1C3B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD650838-369C-4EDD-895B-F154C2A28F7B}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily" sheetId="1" r:id="rId1"/>
     <sheet name="Hourly" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -71,8 +90,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,13 +154,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -179,7 +206,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -213,6 +240,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -247,9 +275,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -422,14 +451,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,12 +508,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B2">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -511,14 +552,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,12 +600,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B2">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -600,12 +641,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B3">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -641,12 +682,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B4">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -682,12 +723,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B5">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -723,12 +764,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B6">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -764,12 +805,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B7">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -805,12 +846,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B8">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -846,12 +887,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B9">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -875,7 +916,7 @@
         <v>62.87</v>
       </c>
       <c r="J9">
-        <v>9.550000000000001</v>
+        <v>9.5500000000000007</v>
       </c>
       <c r="K9">
         <v>8.34</v>
@@ -887,12 +928,12 @@
         <v>7.39</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B10">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -928,12 +969,12 @@
         <v>45.94</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B11">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -954,7 +995,7 @@
         <v>254.42</v>
       </c>
       <c r="I11">
-        <v>639.5700000000001</v>
+        <v>639.57000000000005</v>
       </c>
       <c r="J11">
         <v>73.03</v>
@@ -963,18 +1004,18 @@
         <v>254.06</v>
       </c>
       <c r="L11">
-        <v>616.83</v>
+        <v>616.83000000000004</v>
       </c>
       <c r="M11">
-        <v>71.31999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>71.319999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B12">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1007,15 +1048,15 @@
         <v>717.77</v>
       </c>
       <c r="M12">
-        <v>85.73999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>85.74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B13">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1039,7 +1080,7 @@
         <v>782.58</v>
       </c>
       <c r="J13">
-        <v>93.84999999999999</v>
+        <v>93.85</v>
       </c>
       <c r="K13">
         <v>455.85</v>
@@ -1048,15 +1089,15 @@
         <v>759.33</v>
       </c>
       <c r="M13">
-        <v>97.43000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <v>97.43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B14">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1092,12 +1133,12 @@
         <v>102.38</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B15">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1130,15 +1171,15 @@
         <v>763.72</v>
       </c>
       <c r="M15">
-        <v>98.90000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>98.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B16">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -1162,7 +1203,7 @@
         <v>746.77</v>
       </c>
       <c r="J16">
-        <v>88.18000000000001</v>
+        <v>88.18</v>
       </c>
       <c r="K16">
         <v>392.43</v>
@@ -1171,15 +1212,15 @@
         <v>725.37</v>
       </c>
       <c r="M16">
-        <v>88.76000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>88.76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B17">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1200,27 +1241,27 @@
         <v>279.02</v>
       </c>
       <c r="I17">
-        <v>662.4400000000001</v>
+        <v>662.44</v>
       </c>
       <c r="J17">
-        <v>76.04000000000001</v>
+        <v>76.040000000000006</v>
       </c>
       <c r="K17">
-        <v>275.97</v>
+        <v>275.97000000000003</v>
       </c>
       <c r="L17">
-        <v>626.3099999999999</v>
+        <v>626.30999999999995</v>
       </c>
       <c r="M17">
         <v>76.53</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B18">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -1256,12 +1297,12 @@
         <v>51.78</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B19">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -1288,7 +1329,7 @@
         <v>14.6</v>
       </c>
       <c r="K19">
-        <v>17.85</v>
+        <v>17.850000000000001</v>
       </c>
       <c r="L19">
         <v>55.3</v>
@@ -1297,12 +1338,12 @@
         <v>12.95</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B20">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -1338,12 +1379,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B21">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
@@ -1379,12 +1420,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B22">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -1420,12 +1461,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B23">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -1461,12 +1502,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B24">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -1502,12 +1543,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>47.2229</v>
+        <v>47.222900000000003</v>
       </c>
       <c r="B25">
-        <v>24.7244</v>
+        <v>24.724399999999999</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>

</xml_diff>